<commit_message>
Zone Macro Fully Functioning
</commit_message>
<xml_diff>
--- a/COWA User Acceptance Testing/Data/Connected Office Test Data.xlsx
+++ b/COWA User Acceptance Testing/Data/Connected Office Test Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a4a3de628364ce06/Documents/GitHub/Project-4---C323---34588353/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a4a3de628364ce06/Documents/GitHub/Project-4---C323---34588353/COWA User Acceptance Testing/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAB8EEF-425E-42A8-A7F1-FF25847C778D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="21420" windowHeight="9880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1520" yWindow="1520" windowWidth="21420" windowHeight="9880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -686,7 +686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -911,7 +911,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1127,7 +1127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243FE4D3-E987-44A9-BA20-E766DD09E091}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added References and Compared Test Data
</commit_message>
<xml_diff>
--- a/COWA User Acceptance Testing/Data/Connected Office Test Data.xlsx
+++ b/COWA User Acceptance Testing/Data/Connected Office Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a4a3de628364ce06/Documents/GitHub/Project-4---C323---34588353/COWA User Acceptance Testing/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAB8EEF-425E-42A8-A7F1-FF25847C778D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{FCAB8EEF-425E-42A8-A7F1-FF25847C778D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0ABB196-5083-4944-85D1-CA46C7D635EE}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1520" yWindow="1520" windowWidth="21420" windowHeight="9880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12410" yWindow="1560" windowWidth="21420" windowHeight="9880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -1128,7 +1128,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1164,13 +1164,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1178,16 +1178,16 @@
         <v>58</v>
       </c>
       <c r="B3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1195,16 +1195,16 @@
         <v>59</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1212,16 +1212,16 @@
         <v>60</v>
       </c>
       <c r="B5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1229,16 +1229,16 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1246,16 +1246,16 @@
         <v>62</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1263,16 +1263,16 @@
         <v>63</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1280,16 +1280,16 @@
         <v>64</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1297,16 +1297,16 @@
         <v>65</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -1314,16 +1314,16 @@
         <v>66</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -1331,16 +1331,16 @@
         <v>67</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -1348,16 +1348,16 @@
         <v>68</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -1365,16 +1365,16 @@
         <v>69</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -1382,16 +1382,16 @@
         <v>70</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1399,16 +1399,16 @@
         <v>48</v>
       </c>
       <c r="B16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1416,16 +1416,16 @@
         <v>49</v>
       </c>
       <c r="B17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1433,16 +1433,16 @@
         <v>50</v>
       </c>
       <c r="B18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1450,16 +1450,16 @@
         <v>51</v>
       </c>
       <c r="B19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1467,16 +1467,16 @@
         <v>52</v>
       </c>
       <c r="B20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1484,16 +1484,16 @@
         <v>53</v>
       </c>
       <c r="B21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1501,16 +1501,16 @@
         <v>54</v>
       </c>
       <c r="B22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1518,16 +1518,16 @@
         <v>55</v>
       </c>
       <c r="B23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1535,16 +1535,16 @@
         <v>56</v>
       </c>
       <c r="B24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>